<commit_message>
Fixed d64/t64 sendLine handling using qstring instead. Fixed up colors in excel sheet.
</commit_message>
<xml_diff>
--- a/rpi2uno2iec_connections.xlsx
+++ b/rpi2uno2iec_connections.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="285" windowWidth="28395" windowHeight="14055"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>DIN 6 PIN (C64)</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>not applicable here</t>
+  </si>
+  <si>
+    <t>GPIO P1-18 (GPIO #24)</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,8 +244,30 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -291,8 +316,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -300,8 +351,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
@@ -318,13 +373,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+  <cellStyles count="11">
+    <cellStyle name="20% - Dekorfärg2" xfId="4" builtinId="34"/>
+    <cellStyle name="20% - Dekorfärg5" xfId="5" builtinId="46"/>
+    <cellStyle name="20% - Dekorfärg6" xfId="6" builtinId="50"/>
+    <cellStyle name="40% - Dekorfärg2" xfId="8" builtinId="35"/>
+    <cellStyle name="brun" xfId="10"/>
+    <cellStyle name="Färg1" xfId="3" builtinId="29"/>
+    <cellStyle name="Färg2" xfId="7" builtinId="33"/>
+    <cellStyle name="Färg3" xfId="9" builtinId="37"/>
+    <cellStyle name="Kontrollcell" xfId="2" builtinId="23"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -334,7 +400,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -621,7 +687,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,7 +716,7 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
@@ -674,10 +740,10 @@
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="18"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="I2" s="16"/>
       <c r="J2" t="s">
         <v>45</v>
       </c>
@@ -694,10 +760,10 @@
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="1" t="s">
         <v>42</v>
       </c>
@@ -714,10 +780,10 @@
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="1" t="s">
         <v>43</v>
       </c>
@@ -734,10 +800,10 @@
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="1" t="s">
         <v>44</v>
       </c>
@@ -758,7 +824,7 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -767,7 +833,7 @@
       <c r="H6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -783,7 +849,7 @@
       <c r="E7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -792,7 +858,7 @@
       <c r="H7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="J7" t="s">
@@ -811,7 +877,7 @@
       <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="21" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="7">
@@ -820,7 +886,7 @@
       <c r="H8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="17" t="s">
         <v>34</v>
       </c>
       <c r="J8" t="s">
@@ -839,7 +905,7 @@
       <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="20" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="7">
@@ -848,7 +914,7 @@
       <c r="H9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="17" t="s">
         <v>35</v>
       </c>
       <c r="J9" t="s">
@@ -867,7 +933,7 @@
       <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="7">
@@ -876,7 +942,7 @@
       <c r="H10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="17" t="s">
         <v>38</v>
       </c>
       <c r="J10" t="s">
@@ -891,12 +957,16 @@
       <c r="E11" s="11">
         <v>4</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="11">
         <v>4</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="J11" t="s">
         <v>33</v>
       </c>
@@ -935,6 +1005,7 @@
     <row r="21" spans="1:1" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Both arduino uno and raspberry pi builds. Lots of changes.
M2I and NativeFS must be completed for any functionality to really work.
Complete interface handlers on both rpi and arduino side, most important.
</commit_message>
<xml_diff>
--- a/rpi2uno2iec_connections.xlsx
+++ b/rpi2uno2iec_connections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>DIN 6 PIN (C64)</t>
   </si>
@@ -57,18 +57,9 @@
     <t>10 ohm in series</t>
   </si>
   <si>
-    <t>PIN #7</t>
-  </si>
-  <si>
-    <t>PIN #3</t>
-  </si>
-  <si>
     <t>PIN #2</t>
   </si>
   <si>
-    <t>PIN #6</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>GND 2</t>
   </si>
   <si>
-    <t>AREF</t>
-  </si>
-  <si>
     <t>&lt;--</t>
   </si>
   <si>
@@ -132,9 +120,6 @@
     <t>3V3Power P1-17</t>
   </si>
   <si>
-    <t>GPIO P1-16 (GPIO #23)</t>
-  </si>
-  <si>
     <t>The PI could at free choice (when application starts) or when uses choose to, reset the arduino board.</t>
   </si>
   <si>
@@ -159,14 +144,44 @@
     <t>not applicable here</t>
   </si>
   <si>
-    <t>GPIO P1-18 (GPIO #24)</t>
+    <t>PIN #13</t>
+  </si>
+  <si>
+    <t>SRQ-IN</t>
+  </si>
+  <si>
+    <t>PIN #12</t>
+  </si>
+  <si>
+    <t>PIN #9</t>
+  </si>
+  <si>
+    <t>PIN #10</t>
+  </si>
+  <si>
+    <t>PIN #11</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>IEC Serial Request  In</t>
+  </si>
+  <si>
+    <t>GPIO P1-16 (BCM GPIO #23)</t>
+  </si>
+  <si>
+    <t>GPIO P1-18 (BCM GPIO #24)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,8 +218,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,18 +273,29 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +376,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -352,17 +385,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="6" quotePrefix="1" applyBorder="1"/>
@@ -376,21 +410,29 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="9" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="10" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="11" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="12" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="12"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="11"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="20% - Dekorfärg2" xfId="4" builtinId="34"/>
     <cellStyle name="20% - Dekorfärg5" xfId="5" builtinId="46"/>
     <cellStyle name="20% - Dekorfärg6" xfId="6" builtinId="50"/>
-    <cellStyle name="40% - Dekorfärg2" xfId="8" builtinId="35"/>
-    <cellStyle name="brun" xfId="10"/>
+    <cellStyle name="brun" xfId="9"/>
+    <cellStyle name="Dålig" xfId="10" builtinId="27"/>
     <cellStyle name="Färg1" xfId="3" builtinId="29"/>
     <cellStyle name="Färg2" xfId="7" builtinId="33"/>
-    <cellStyle name="Färg3" xfId="9" builtinId="37"/>
+    <cellStyle name="Färg3" xfId="8" builtinId="37"/>
+    <cellStyle name="Grå" xfId="11"/>
     <cellStyle name="Kontrollcell" xfId="2" builtinId="23"/>
+    <cellStyle name="Lila" xfId="12"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -684,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,293 +758,319 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>31</v>
+      <c r="J1" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="C2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="A3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="H7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="I7" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="17" t="s">
+      <c r="D10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="6">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="10">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="10">
+        <v>4</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A20" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4">
-        <v>2</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="7">
-        <v>3</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="11">
-        <v>4</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="11">
-        <v>4</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1">
-      <c r="A19" s="13" t="s">
+    <row r="21" spans="1:1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A21" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A20" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" thickTop="1"/>
+    <row r="22" spans="1:1" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Supporting directory listing, first attempt. Now also added interface for media info. None implemented yet. Fixed the connection schema in the excel sheet. Added some notes for testing.
</commit_message>
<xml_diff>
--- a/rpi2uno2iec_connections.xlsx
+++ b/rpi2uno2iec_connections.xlsx
@@ -144,24 +144,9 @@
     <t>not applicable here</t>
   </si>
   <si>
-    <t>PIN #13</t>
-  </si>
-  <si>
     <t>SRQ-IN</t>
   </si>
   <si>
-    <t>PIN #12</t>
-  </si>
-  <si>
-    <t>PIN #9</t>
-  </si>
-  <si>
-    <t>PIN #10</t>
-  </si>
-  <si>
-    <t>PIN #11</t>
-  </si>
-  <si>
     <t>5V</t>
   </si>
   <si>
@@ -175,6 +160,21 @@
   </si>
   <si>
     <t>GPIO P1-18 (BCM GPIO #24)</t>
+  </si>
+  <si>
+    <t>PIN #3</t>
+  </si>
+  <si>
+    <t>PIN #4</t>
+  </si>
+  <si>
+    <t>PIN #5</t>
+  </si>
+  <si>
+    <t>PIN #6</t>
+  </si>
+  <si>
+    <t>PIN #7</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -792,13 +792,13 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -807,7 +807,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
       <c r="J3" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
@@ -818,7 +818,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -838,7 +838,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -903,7 +903,7 @@
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>6</v>
@@ -1005,7 +1005,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
@@ -1018,22 +1018,22 @@
         <v>13</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" s="10">
         <v>4</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G12" s="10">
         <v>4</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
         <v>29</v>

</xml_diff>